<commit_message>
Small, inconsequential changes to data sets.
</commit_message>
<xml_diff>
--- a/Data/list of APA-journals.xlsx
+++ b/Data/list of APA-journals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EliseSchramkowski\Documents\GitHub\thesis\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14361C6F-4F3F-4C0B-BC63-101DFB43E47B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D09F0F-5F0B-4A35-BF4D-62F72B625EE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="936" yWindow="1908" windowWidth="14508" windowHeight="14772" xr2:uid="{02E59939-79B7-4D13-B8FC-A3ADFAE9CF57}"/>
   </bookViews>
@@ -697,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E11D862E-5D70-4618-980A-1E1FFC3E34BB}">
   <dimension ref="A1:A102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="A95" sqref="A95:A102"/>
+    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
+      <selection activeCell="A93" sqref="A93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>